<commit_message>
commit the properties implementation
</commit_message>
<xml_diff>
--- a/exceltestdata/TC001.xlsx
+++ b/exceltestdata/TC001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Eclipse\eclipse-workspace\MavenProject\exceltestdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B0C47D8-07EE-478A-A692-DF72BBE83583}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC81DF78-6BC5-41CD-8EE3-5E2E62A28F9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3015" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,10 @@
     <t>password</t>
   </si>
   <si>
-    <t>India$321</t>
-  </si>
-  <si>
     <t>hari.radhakrishnan@qeagle.com</t>
+  </si>
+  <si>
+    <t>India$4321</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,10 +410,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -425,10 +425,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
       <c r="C3" t="s">
         <v>2</v>

</xml_diff>